<commit_message>
Please provide the file changes to generate a commit message.
</commit_message>
<xml_diff>
--- a/COMISSÕES POR REGIAO.xlsx
+++ b/COMISSÕES POR REGIAO.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\APRENDIZADO APP\MEDIÇÕES\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65F3B8E2-5826-44BF-8FA5-18A1542E83CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C3056CA-8312-4B49-B294-4EA711548896}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="498" activeTab="5" xr2:uid="{8E7E61FA-AA35-49DA-A0A0-B5261C3AB08E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="498" xr2:uid="{8E7E61FA-AA35-49DA-A0A0-B5261C3AB08E}"/>
   </bookViews>
   <sheets>
     <sheet name="BAIXADA" sheetId="1" r:id="rId1"/>
@@ -2284,7 +2284,7 @@
     <xf numFmtId="167" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="104">
+  <cellXfs count="102">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2540,17 +2540,13 @@
     <xf numFmtId="1" fontId="25" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="13" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="13" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="44" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="44" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="62">
     <cellStyle name="20% - Ênfase1" xfId="12" builtinId="30" customBuiltin="1"/>
@@ -4253,7 +4249,13 @@
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{219523AD-7502-4955-9305-1317053F81AC}" name="TBL_AUX_COMISSAO" displayName="TBL_AUX_COMISSAO" ref="A1:F130" totalsRowShown="0" headerRowDxfId="59" dataDxfId="57" headerRowBorderDxfId="58" tableBorderDxfId="56" totalsRowBorderDxfId="55">
-  <autoFilter ref="A1:F130" xr:uid="{219523AD-7502-4955-9305-1317053F81AC}"/>
+  <autoFilter ref="A1:F130" xr:uid="{219523AD-7502-4955-9305-1317053F81AC}">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="330001/001081/2025"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F121">
     <sortCondition ref="A1:A124"/>
   </sortState>
@@ -4587,10 +4589,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69DBBD80-2FBA-444A-B434-052B47DD7E2E}">
   <sheetPr codeName="Planilha1"/>
-  <dimension ref="A1:G62"/>
+  <dimension ref="A1:S62"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="S5" sqref="S5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4605,18 +4607,18 @@
     <col min="8" max="8" width="12.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4"/>
-      <c r="B1" s="99" t="s">
+      <c r="B1" s="100" t="s">
         <v>142</v>
       </c>
-      <c r="C1" s="100"/>
-      <c r="D1" s="100"/>
-      <c r="E1" s="100"/>
-      <c r="F1" s="100"/>
-      <c r="G1" s="100"/>
-    </row>
-    <row r="2" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="C1" s="101"/>
+      <c r="D1" s="101"/>
+      <c r="E1" s="101"/>
+      <c r="F1" s="101"/>
+      <c r="G1" s="101"/>
+    </row>
+    <row r="2" spans="1:19" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B2" s="41" t="s">
         <v>35</v>
       </c>
@@ -4636,7 +4638,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -4659,7 +4661,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -4682,7 +4684,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -4704,8 +4706,12 @@
       <c r="G5" s="7" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="S5">
+        <f>1331-2.43</f>
+        <v>1328.57</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -4728,7 +4734,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -4751,7 +4757,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -4774,7 +4780,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -4797,7 +4803,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -4820,7 +4826,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -4843,7 +4849,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -4866,7 +4872,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -4889,7 +4895,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -4912,7 +4918,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -4935,7 +4941,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -5787,14 +5793,14 @@
   <sheetData>
     <row r="1" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4"/>
-      <c r="B1" s="99" t="s">
+      <c r="B1" s="100" t="s">
         <v>122</v>
       </c>
-      <c r="C1" s="100"/>
-      <c r="D1" s="100"/>
-      <c r="E1" s="100"/>
-      <c r="F1" s="100"/>
-      <c r="G1" s="100"/>
+      <c r="C1" s="101"/>
+      <c r="D1" s="101"/>
+      <c r="E1" s="101"/>
+      <c r="F1" s="101"/>
+      <c r="G1" s="101"/>
     </row>
     <row r="2" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A2" s="4"/>
@@ -6301,14 +6307,14 @@
   <sheetData>
     <row r="1" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4"/>
-      <c r="B1" s="99" t="s">
+      <c r="B1" s="100" t="s">
         <v>131</v>
       </c>
-      <c r="C1" s="100"/>
-      <c r="D1" s="100"/>
-      <c r="E1" s="100"/>
-      <c r="F1" s="100"/>
-      <c r="G1" s="100"/>
+      <c r="C1" s="101"/>
+      <c r="D1" s="101"/>
+      <c r="E1" s="101"/>
+      <c r="F1" s="101"/>
+      <c r="G1" s="101"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="4"/>
@@ -7065,14 +7071,14 @@
   <sheetData>
     <row r="1" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4"/>
-      <c r="B1" s="99" t="s">
+      <c r="B1" s="100" t="s">
         <v>271</v>
       </c>
-      <c r="C1" s="100"/>
-      <c r="D1" s="100"/>
-      <c r="E1" s="100"/>
-      <c r="F1" s="100"/>
-      <c r="G1" s="100"/>
+      <c r="C1" s="101"/>
+      <c r="D1" s="101"/>
+      <c r="E1" s="101"/>
+      <c r="F1" s="101"/>
+      <c r="G1" s="101"/>
     </row>
     <row r="2" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A2" s="4"/>
@@ -7286,7 +7292,7 @@
       <c r="B11" s="32" t="s">
         <v>345</v>
       </c>
-      <c r="C11" s="101" t="s">
+      <c r="C11" s="99" t="s">
         <v>300</v>
       </c>
       <c r="D11" s="25" t="s">
@@ -7487,14 +7493,14 @@
   <sheetData>
     <row r="1" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4"/>
-      <c r="B1" s="99" t="s">
+      <c r="B1" s="100" t="s">
         <v>208</v>
       </c>
-      <c r="C1" s="100"/>
-      <c r="D1" s="100"/>
-      <c r="E1" s="100"/>
-      <c r="F1" s="100"/>
-      <c r="G1" s="100"/>
+      <c r="C1" s="101"/>
+      <c r="D1" s="101"/>
+      <c r="E1" s="101"/>
+      <c r="F1" s="101"/>
+      <c r="G1" s="101"/>
     </row>
     <row r="2" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A2" s="4"/>
@@ -8109,7 +8115,7 @@
   <sheetPr codeName="Planilha4"/>
   <dimension ref="A1:F130"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A130" sqref="A130"/>
     </sheetView>
   </sheetViews>
@@ -8144,7 +8150,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>189</v>
       </c>
@@ -8178,7 +8184,7 @@
         <v>ESPECIAIS</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>106</v>
       </c>
@@ -8205,7 +8211,7 @@
         <v>CIVIS</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>52</v>
       </c>
@@ -8232,7 +8238,7 @@
         <v>CIVIS</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>102</v>
       </c>
@@ -8259,7 +8265,7 @@
         <v>CIVIS</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>213</v>
       </c>
@@ -8286,7 +8292,7 @@
         <v>CIVIS</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>176</v>
       </c>
@@ -8313,7 +8319,7 @@
         <v>CIVIS</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>181</v>
       </c>
@@ -8340,7 +8346,7 @@
         <v>ESPECIAIS</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>209</v>
       </c>
@@ -8367,7 +8373,7 @@
         <v>CIVIS</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>168</v>
       </c>
@@ -8394,7 +8400,7 @@
         <v>CIVIS</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>182</v>
       </c>
@@ -8421,7 +8427,7 @@
         <v>ESPECIAIS</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>212</v>
       </c>
@@ -8448,7 +8454,7 @@
         <v>CIVIS</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>119</v>
       </c>
@@ -8475,7 +8481,7 @@
         <v>CIVIS</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>262</v>
       </c>
@@ -8502,7 +8508,7 @@
         <v>CIVIS</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>172</v>
       </c>
@@ -8529,7 +8535,7 @@
         <v>CIVIS</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>80</v>
       </c>
@@ -8556,7 +8562,7 @@
         <v>CIVIS</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>250</v>
       </c>
@@ -8583,7 +8589,7 @@
         <v>CIVIS</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>113</v>
       </c>
@@ -8610,7 +8616,7 @@
         <v>CIVIS</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>165</v>
       </c>
@@ -8637,7 +8643,7 @@
         <v>CIVIS</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>10</v>
       </c>
@@ -8664,7 +8670,7 @@
         <v>CIVIS</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>79</v>
       </c>
@@ -8691,7 +8697,7 @@
         <v>CIVIS</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>132</v>
       </c>
@@ -8718,7 +8724,7 @@
         <v>CIVIS</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>152</v>
       </c>
@@ -8745,7 +8751,7 @@
         <v>CIVIS</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>219</v>
       </c>
@@ -8772,7 +8778,7 @@
         <v>CIVIS</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>169</v>
       </c>
@@ -8799,7 +8805,7 @@
         <v>CIVIS</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>116</v>
       </c>
@@ -8826,7 +8832,7 @@
         <v>CIVIS</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>78</v>
       </c>
@@ -8853,7 +8859,7 @@
         <v>CIVIS</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>145</v>
       </c>
@@ -8880,7 +8886,7 @@
         <v>CIVIS</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>21</v>
       </c>
@@ -8907,7 +8913,7 @@
         <v>CIVIS</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>170</v>
       </c>
@@ -8934,7 +8940,7 @@
         <v>CIVIS</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>51</v>
       </c>
@@ -8961,7 +8967,7 @@
         <v>CIVIS</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>240</v>
       </c>
@@ -8988,7 +8994,7 @@
         <v>ESPECIAIS</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>233</v>
       </c>
@@ -9015,7 +9021,7 @@
         <v>ESPECIAIS</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>269</v>
       </c>
@@ -9049,7 +9055,7 @@
         <v>ESPECIAIS</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
         <v>171</v>
       </c>
@@ -9076,7 +9082,7 @@
         <v>CIVIS</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
         <v>274</v>
       </c>
@@ -9103,7 +9109,7 @@
         <v>ESPECIAIS</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
         <v>221</v>
       </c>
@@ -9130,7 +9136,7 @@
         <v>CIVIS</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
         <v>265</v>
       </c>
@@ -9157,7 +9163,7 @@
         <v>CIVIS</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
         <v>174</v>
       </c>
@@ -9184,7 +9190,7 @@
         <v>CIVIS</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
         <v>96</v>
       </c>
@@ -9238,7 +9244,7 @@
         <v>CONTINGENCIA</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
         <v>266</v>
       </c>
@@ -9265,7 +9271,7 @@
         <v>CONTINGENCIA</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
         <v>245</v>
       </c>
@@ -9292,7 +9298,7 @@
         <v>CONTINGENCIA</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
         <v>277</v>
       </c>
@@ -9319,7 +9325,7 @@
         <v>CIVIS</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
         <v>261</v>
       </c>
@@ -9346,7 +9352,7 @@
         <v>CIVIS</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
         <v>211</v>
       </c>
@@ -9373,7 +9379,7 @@
         <v>CIVIS</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
         <v>223</v>
       </c>
@@ -9400,7 +9406,7 @@
         <v>CIVIS</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
         <v>155</v>
       </c>
@@ -9427,7 +9433,7 @@
         <v>CIVIS</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
         <v>153</v>
       </c>
@@ -9454,7 +9460,7 @@
         <v>CIVIS</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
         <v>104</v>
       </c>
@@ -9481,7 +9487,7 @@
         <v>CIVIS</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
         <v>154</v>
       </c>
@@ -9508,7 +9514,7 @@
         <v>CIVIS</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
         <v>120</v>
       </c>
@@ -9535,7 +9541,7 @@
         <v>CIVIS</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
         <v>164</v>
       </c>
@@ -9562,7 +9568,7 @@
         <v>CIVIS</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
         <v>151</v>
       </c>
@@ -9589,7 +9595,7 @@
         <v>CIVIS</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
         <v>128</v>
       </c>
@@ -9616,7 +9622,7 @@
         <v>CIVIS</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
         <v>259</v>
       </c>
@@ -9643,7 +9649,7 @@
         <v>CONTINGENCIA</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
         <v>81</v>
       </c>
@@ -9670,7 +9676,7 @@
         <v>CIVIS</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
         <v>161</v>
       </c>
@@ -9697,7 +9703,7 @@
         <v>CIVIS</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
         <v>83</v>
       </c>
@@ -9724,7 +9730,7 @@
         <v>CIVIS</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
         <v>30</v>
       </c>
@@ -9751,7 +9757,7 @@
         <v>CIVIS</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
         <v>136</v>
       </c>
@@ -9778,7 +9784,7 @@
         <v>CIVIS</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
         <v>162</v>
       </c>
@@ -9805,7 +9811,7 @@
         <v>CIVIS</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
         <v>121</v>
       </c>
@@ -9832,7 +9838,7 @@
         <v>CIVIS</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
         <v>156</v>
       </c>
@@ -9859,7 +9865,7 @@
         <v>CIVIS</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="s">
         <v>134</v>
       </c>
@@ -9886,7 +9892,7 @@
         <v>CIVIS</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66" s="3" t="s">
         <v>157</v>
       </c>
@@ -9920,7 +9926,7 @@
         <v>CIVIS</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67" s="3" t="s">
         <v>82</v>
       </c>
@@ -9947,7 +9953,7 @@
         <v>CIVIS</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" s="3" t="s">
         <v>8</v>
       </c>
@@ -9974,7 +9980,7 @@
         <v>CIVIS</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69" s="3" t="s">
         <v>16</v>
       </c>
@@ -10001,7 +10007,7 @@
         <v>CIVIS</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70" s="3" t="s">
         <v>17</v>
       </c>
@@ -10028,7 +10034,7 @@
         <v>CIVIS</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71" s="3" t="s">
         <v>19</v>
       </c>
@@ -10055,7 +10061,7 @@
         <v>CIVIS</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72" s="3" t="s">
         <v>135</v>
       </c>
@@ -10082,7 +10088,7 @@
         <v>CIVIS</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73" s="3" t="s">
         <v>158</v>
       </c>
@@ -10109,7 +10115,7 @@
         <v>CIVIS</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74" s="3" t="s">
         <v>159</v>
       </c>
@@ -10136,7 +10142,7 @@
         <v>CIVIS</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A75" s="3" t="s">
         <v>160</v>
       </c>
@@ -10163,7 +10169,7 @@
         <v>CIVIS</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A76" s="3" t="s">
         <v>7</v>
       </c>
@@ -10190,7 +10196,7 @@
         <v>CIVIS</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77" s="3" t="s">
         <v>24</v>
       </c>
@@ -10217,7 +10223,7 @@
         <v>CIVIS</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78" s="3" t="s">
         <v>94</v>
       </c>
@@ -10244,7 +10250,7 @@
         <v>CIVIS</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A79" s="3" t="s">
         <v>26</v>
       </c>
@@ -10271,7 +10277,7 @@
         <v>CIVIS</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80" s="3" t="s">
         <v>22</v>
       </c>
@@ -10298,7 +10304,7 @@
         <v>CIVIS</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A81" s="3" t="s">
         <v>133</v>
       </c>
@@ -10325,7 +10331,7 @@
         <v>CIVIS</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A82" s="3" t="s">
         <v>5</v>
       </c>
@@ -10352,7 +10358,7 @@
         <v>CIVIS</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A83" s="3" t="s">
         <v>27</v>
       </c>
@@ -10379,7 +10385,7 @@
         <v>CIVIS</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A84" s="3" t="s">
         <v>34</v>
       </c>
@@ -10406,7 +10412,7 @@
         <v>CIVIS</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A85" s="3" t="s">
         <v>0</v>
       </c>
@@ -10433,7 +10439,7 @@
         <v>CIVIS</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A86" s="3" t="s">
         <v>32</v>
       </c>
@@ -10460,7 +10466,7 @@
         <v>CIVIS</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A87" s="3" t="s">
         <v>147</v>
       </c>
@@ -10487,7 +10493,7 @@
         <v>CIVIS</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A88" s="3" t="s">
         <v>29</v>
       </c>
@@ -10514,7 +10520,7 @@
         <v>CIVIS</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A89" s="3" t="s">
         <v>14</v>
       </c>
@@ -10541,7 +10547,7 @@
         <v>CIVIS</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A90" s="3" t="s">
         <v>12</v>
       </c>
@@ -10568,7 +10574,7 @@
         <v>CIVIS</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A91" s="3" t="s">
         <v>111</v>
       </c>
@@ -10595,7 +10601,7 @@
         <v>CIVIS</v>
       </c>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A92" s="3" t="s">
         <v>146</v>
       </c>
@@ -10622,7 +10628,7 @@
         <v>CIVIS</v>
       </c>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A93" s="3" t="s">
         <v>236</v>
       </c>
@@ -10649,7 +10655,7 @@
         <v>CONTINGENCIA</v>
       </c>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A94" s="3" t="s">
         <v>242</v>
       </c>
@@ -10676,7 +10682,7 @@
         <v>CONTINGENCIA</v>
       </c>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A95" s="3" t="s">
         <v>2</v>
       </c>
@@ -10703,7 +10709,7 @@
         <v>CIVIS</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A96" s="3" t="s">
         <v>248</v>
       </c>
@@ -10730,7 +10736,7 @@
         <v>CONTINGENCIA</v>
       </c>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A97" s="3" t="s">
         <v>4</v>
       </c>
@@ -10757,7 +10763,7 @@
         <v>CIVIS</v>
       </c>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A98" s="3" t="s">
         <v>173</v>
       </c>
@@ -10791,7 +10797,7 @@
         <v>CIVIS</v>
       </c>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A99" s="3" t="s">
         <v>115</v>
       </c>
@@ -10818,7 +10824,7 @@
         <v>CIVIS</v>
       </c>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A100" s="3" t="s">
         <v>175</v>
       </c>
@@ -10845,7 +10851,7 @@
         <v>CIVIS</v>
       </c>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A101" s="3" t="s">
         <v>226</v>
       </c>
@@ -10872,7 +10878,7 @@
         <v>ESPECIAIS</v>
       </c>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A102" s="3" t="s">
         <v>180</v>
       </c>
@@ -10899,7 +10905,7 @@
         <v>ESPECIAIS</v>
       </c>
     </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A103" s="3" t="s">
         <v>215</v>
       </c>
@@ -10926,7 +10932,7 @@
         <v>ESPECIAIS</v>
       </c>
     </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A104" s="3" t="s">
         <v>256</v>
       </c>
@@ -10953,7 +10959,7 @@
         <v>ESPECIAIS</v>
       </c>
     </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A105" s="3" t="s">
         <v>163</v>
       </c>
@@ -10980,7 +10986,7 @@
         <v>CIVIS</v>
       </c>
     </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A106" s="3" t="s">
         <v>143</v>
       </c>
@@ -11007,7 +11013,7 @@
         <v>CIVIS</v>
       </c>
     </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A107" s="3" t="s">
         <v>183</v>
       </c>
@@ -11034,7 +11040,7 @@
         <v>ESPECIAIS</v>
       </c>
     </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A108" s="3" t="s">
         <v>191</v>
       </c>
@@ -11061,7 +11067,7 @@
         <v>ESPECIAIS</v>
       </c>
     </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A109" s="3" t="s">
         <v>218</v>
       </c>
@@ -11088,7 +11094,7 @@
         <v>CIVIS</v>
       </c>
     </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A110" s="3" t="s">
         <v>217</v>
       </c>
@@ -11115,7 +11121,7 @@
         <v>CIVIS</v>
       </c>
     </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A111" s="3" t="s">
         <v>184</v>
       </c>
@@ -11142,7 +11148,7 @@
         <v>ESPECIAIS</v>
       </c>
     </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A112" s="3" t="s">
         <v>185</v>
       </c>
@@ -11169,7 +11175,7 @@
         <v>ESPECIAIS</v>
       </c>
     </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A113" s="3" t="s">
         <v>186</v>
       </c>
@@ -11196,7 +11202,7 @@
         <v>ESPECIAIS</v>
       </c>
     </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A114" s="3" t="s">
         <v>255</v>
       </c>
@@ -11223,7 +11229,7 @@
         <v>ESPECIAIS</v>
       </c>
     </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A115" s="3" t="s">
         <v>257</v>
       </c>
@@ -11250,7 +11256,7 @@
         <v>ESPECIAIS</v>
       </c>
     </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A116" s="3" t="s">
         <v>187</v>
       </c>
@@ -11277,7 +11283,7 @@
         <v>ESPECIAIS</v>
       </c>
     </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A117" s="3" t="s">
         <v>188</v>
       </c>
@@ -11304,7 +11310,7 @@
         <v>ESPECIAIS</v>
       </c>
     </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A118" s="3" t="s">
         <v>230</v>
       </c>
@@ -11331,7 +11337,7 @@
         <v>CIVIS</v>
       </c>
     </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A119" s="3" t="s">
         <v>251</v>
       </c>
@@ -11358,7 +11364,7 @@
         <v>CIVIS</v>
       </c>
     </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A120" s="3" t="s">
         <v>144</v>
       </c>
@@ -11385,7 +11391,7 @@
         <v>ESPECIAIS</v>
       </c>
     </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A121" s="3" t="s">
         <v>281</v>
       </c>
@@ -11412,7 +11418,7 @@
         <v>CONTINGENCIA</v>
       </c>
     </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A122" s="3" t="s">
         <v>190</v>
       </c>
@@ -11439,7 +11445,7 @@
         <v>ESPECIAIS</v>
       </c>
     </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A123" s="3" t="s">
         <v>192</v>
       </c>
@@ -11466,7 +11472,7 @@
         <v>ESPECIAIS</v>
       </c>
     </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A124" s="3" t="s">
         <v>224</v>
       </c>
@@ -11493,7 +11499,7 @@
         <v>ESPECIAIS</v>
       </c>
     </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A125" s="16" t="s">
         <v>287</v>
       </c>
@@ -11520,7 +11526,7 @@
         <v>CIVIS</v>
       </c>
     </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A126" s="24" t="s">
         <v>289</v>
       </c>
@@ -11547,7 +11553,7 @@
         <v>CIVIS</v>
       </c>
     </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A127" s="24" t="s">
         <v>339</v>
       </c>
@@ -11574,7 +11580,7 @@
         <v>CIVIS</v>
       </c>
     </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A128" s="24" t="s">
         <v>341</v>
       </c>
@@ -11601,7 +11607,7 @@
         <v>CIVIS</v>
       </c>
     </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A129" s="24" t="s">
         <v>343</v>
       </c>
@@ -11628,11 +11634,11 @@
         <v>ESPECIAIS</v>
       </c>
     </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A130" s="24" t="s">
         <v>345</v>
       </c>
-      <c r="B130" s="102" t="str">
+      <c r="B130" s="93" t="str">
         <f ca="1">UPPER(TRIM(UPPER(IFERROR(VLOOKUP(A130,INDIRECT("'BAIXADA'!$B$3:$I$51"),3,FALSE),
 IFERROR(VLOOKUP(A130,INDIRECT("'NORTE'!$B$3:$I$21"),3,FALSE),
 IFERROR(VLOOKUP(A130,INDIRECT("'SUL'!$B$3:$I$31"),3,FALSE),
@@ -11640,7 +11646,7 @@
 IFERROR(VLOOKUP(A130,INDIRECT("'ESPECIAIS'!$B$3:$I$27"),3,FALSE),""))))))))</f>
         <v>GISELLE G. FONSECA</v>
       </c>
-      <c r="C130" s="102" t="str">
+      <c r="C130" s="93" t="str">
         <f ca="1">IF(OR(B130="CARLOS FERNANDES", B130="GISELLE G. FONSECA"), "BAIXADA",
  IF(OR(B130="ISADORA ROSALINO", B130="JEHNIFFER PIRES"), "NORTE",
  IF(OR(B130="LUIZ FILHO", B130="MARCUS", B130="JAQUELINE PASTÓRIO"), "SUL",
@@ -11648,7 +11654,7 @@
         <v>BAIXADA</v>
       </c>
       <c r="D130" s="86"/>
-      <c r="E130" s="103" t="str">
+      <c r="E130" s="86" t="str">
         <f>UPPER(TRIM(IFERROR(VLOOKUP(TBL_AUX_COMISSAO[[#This Row],[SEI]], TBL_BAIXADA[[SEI]:[STATUS]],4,FALSE),
  IFERROR(VLOOKUP(TBL_AUX_COMISSAO[[#This Row],[SEI]], Tabela2[[SEI]:[STATUS]],4,FALSE),
  IFERROR(VLOOKUP(TBL_AUX_COMISSAO[[#This Row],[SEI]], Tabela3[[SEI]:[STATUS]],4,FALSE),
@@ -11656,7 +11662,7 @@
  IFERROR(VLOOKUP(TBL_AUX_COMISSAO[[#This Row],[SEI]], Tabela5[[SEI]:[STATUS]],4,FALSE),"Valor não encontrado")))))))</f>
         <v>EXECUÇÃO</v>
       </c>
-      <c r="F130" s="103" t="str">
+      <c r="F130" s="86" t="str">
         <f>UPPER(IF(SUM(COUNTIF(BAIXADA!B:B,A130),COUNTIF(NORTE!B:B,A130),COUNTIF(SUL!B:B,A130))&gt;0,"CIVIS",
 IF(COUNTIF(CONTIGENCIA!B:B,A130)&gt;0,"CONTINGENCIA",IF(COUNTIF(ESPECIAIS!B:B,A130)&gt;0,"ESPECIAIS",""))))</f>
         <v>CONTINGENCIA</v>

</xml_diff>